<commit_message>
final ready go p.s dont do drugs. please
</commit_message>
<xml_diff>
--- a/Count_by_demo.xlsx
+++ b/Count_by_demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mirun\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44492F94-BD46-4BAB-9645-EDD850EE387F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8ACB2C-EAF2-4FCC-914C-632E290A9EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C174D4C1-13A1-4581-8BA1-103CBD0A64D2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="21">
   <si>
     <t>  American Indian or Alaska Native (Non-Hispanic)</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>Year</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
 </sst>
 </file>
@@ -482,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{917133E2-24F2-4584-98F9-E8784AF39936}">
   <dimension ref="A1:Y85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1484,8 +1481,8 @@
       <c r="D17" s="1">
         <v>4.5</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>21</v>
+      <c r="E17" s="1">
+        <v>5.0999999999999996</v>
       </c>
       <c r="F17" s="1">
         <v>5.6</v>

</xml_diff>